<commit_message>
Salvamento de dados ao sair
</commit_message>
<xml_diff>
--- a/Sprint-4/Product Backlog-Burndown.xlsx
+++ b/Sprint-4/Product Backlog-Burndown.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="108">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>Criar Tela Cadastro Adm</t>
+  </si>
+  <si>
+    <t>Para gerenciar o sistema, o administrador deverá fazer o login com seus dados</t>
+  </si>
+  <si>
+    <t>A tela de login será apresentada ao entrar no software. O login é uma necessidade apenas para administradores.</t>
   </si>
 </sst>
 </file>
@@ -699,40 +705,43 @@
     <xf numFmtId="4" fontId="13" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -751,9 +760,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1677,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1693,14 +1699,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1805,10 +1811,10 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1838,8 +1844,8 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="21" t="s">
         <v>55</v>
       </c>
@@ -1867,8 +1873,8 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="22" t="s">
         <v>56</v>
       </c>
@@ -1896,10 +1902,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1929,8 +1935,8 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="3" t="s">
         <v>44</v>
       </c>
@@ -1958,8 +1964,8 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
@@ -1987,8 +1993,8 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
@@ -2016,8 +2022,8 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
@@ -2045,8 +2051,8 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
@@ -2074,8 +2080,8 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="6" t="s">
         <v>43</v>
       </c>
@@ -2103,8 +2109,8 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
@@ -2132,10 +2138,10 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="30" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -2165,8 +2171,8 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2194,8 +2200,8 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="6" t="s">
         <v>60</v>
       </c>
@@ -2223,8 +2229,8 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="6" t="s">
         <v>61</v>
       </c>
@@ -2252,8 +2258,8 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="6" t="s">
         <v>62</v>
       </c>
@@ -2281,8 +2287,8 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="6" t="s">
         <v>63</v>
       </c>
@@ -2310,8 +2316,8 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="6" t="s">
         <v>64</v>
       </c>
@@ -2339,8 +2345,8 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="6" t="s">
         <v>65</v>
       </c>
@@ -2368,8 +2374,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="4" t="s">
         <v>66</v>
       </c>
@@ -2397,10 +2403,10 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="30" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2430,8 +2436,8 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="23" t="s">
         <v>76</v>
       </c>
@@ -2459,8 +2465,8 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="23" t="s">
         <v>77</v>
       </c>
@@ -2488,10 +2494,10 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="30" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="23" t="s">
@@ -2521,8 +2527,8 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="6" t="s">
         <v>70</v>
       </c>
@@ -2550,8 +2556,8 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="6" t="s">
         <v>71</v>
       </c>
@@ -2579,8 +2585,8 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="24" t="s">
         <v>73</v>
       </c>
@@ -2608,8 +2614,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="24" t="s">
         <v>72</v>
       </c>
@@ -2637,10 +2643,10 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="30" t="s">
         <v>102</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -2666,8 +2672,8 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="24" t="s">
         <v>104</v>
       </c>
@@ -2691,8 +2697,8 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="24" t="s">
         <v>105</v>
       </c>
@@ -2716,10 +2722,10 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="30" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -2732,8 +2738,8 @@
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="6" t="s">
         <v>96</v>
       </c>
@@ -2744,8 +2750,8 @@
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="6" t="s">
         <v>97</v>
       </c>
@@ -2756,10 +2762,10 @@
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="30" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -2772,8 +2778,8 @@
       <c r="F39" s="6"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="6" t="s">
         <v>99</v>
       </c>
@@ -2784,8 +2790,8 @@
       <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="3" t="s">
         <v>100</v>
       </c>
@@ -2843,9 +2849,13 @@
       <c r="E45" s="5"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+    <row r="46" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="C46" s="6"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
@@ -3050,11 +3060,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="B39:B41"/>
@@ -3067,6 +3072,11 @@
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3102,20 +3112,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="1"/>
@@ -3130,22 +3140,22 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="39" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="46" t="s">
@@ -3154,16 +3164,16 @@
       <c r="H2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="39" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="1"/>
@@ -3178,18 +3188,18 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="39"/>
       <c r="G3" s="46"/>
       <c r="H3" s="46"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3377,22 +3387,22 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="17" t="s">
         <v>9</v>
       </c>
@@ -3411,10 +3421,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="40">
+      <c r="A9" s="41">
         <v>50</v>
       </c>
-      <c r="B9" s="40"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="15">
         <f>SUMIF('Product Backlog'!F:F,1,'Product Backlog'!E:E)</f>
         <v>35</v>
@@ -3476,6 +3486,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:L8"/>
@@ -3492,7 +3503,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>

<commit_message>
Atualização Código e Documentos Sprint 4
</commit_message>
<xml_diff>
--- a/Sprint-4/Product Backlog-Burndown.xlsx
+++ b/Sprint-4/Product Backlog-Burndown.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno\Downloads\adocao6\Sprint-4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8145" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Product Burndown" sheetId="2" r:id="rId2"/>
     <sheet name="Lista de tarefas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -274,9 +264,6 @@
     <t>O usuário tem a opção de fechar o software. Ao fechar o software, se deve ter garantia que nenhum dado seja perdido</t>
   </si>
   <si>
-    <t>Após o cadastro do animal, deverá ser fornecido a opção para mudar os dados cadastrados de cada animal.</t>
-  </si>
-  <si>
     <t>É necessario ter um controle dos candidatos para adoção, então se deve criar uma tela de visualização dos candidatos</t>
   </si>
   <si>
@@ -304,9 +291,6 @@
     <t>Ao clicar em fechar, será apresentado uma caixa de confirmação da ação, perguntando se deseja realmente sair.</t>
   </si>
   <si>
-    <t>Será mostrado a lista de animais, e ao clicar no animal em que se deseja fazer a alteração, a tela de edição será mostrada.</t>
-  </si>
-  <si>
     <t>Haverá uma lista com todos os usuários que conseguiram ou não realizar a adoção.</t>
   </si>
   <si>
@@ -353,12 +337,57 @@
   </si>
   <si>
     <t>Criar classe sessao</t>
+  </si>
+  <si>
+    <t>Melhorar as telas de cadastro, visualização e edição de dados</t>
+  </si>
+  <si>
+    <t>O sistema deverá abrir apenas uma Janela Principal, e os cadastros e visualizações serão definidas como JInternalFrame para que todo o espaço seja aproveitado.</t>
+  </si>
+  <si>
+    <t>Estudar e Implementar a Biblioteca JInternalFrame</t>
+  </si>
+  <si>
+    <t>Atualizar Telas para JInternalFrame</t>
+  </si>
+  <si>
+    <t>Desejo que o Sistema forneça uma opção para alteração dos dados de animais cadastrados</t>
+  </si>
+  <si>
+    <t>O Sistema vai possuir uma opção de alteração na TelaPrincipal, com acesso a alteração dos dados dos animais</t>
+  </si>
+  <si>
+    <t>Tratar o Evento de Alteração de Dados</t>
+  </si>
+  <si>
+    <t>Busca e Visualização de Dados</t>
+  </si>
+  <si>
+    <t>Salvar Alterações no Banco de Dados</t>
+  </si>
+  <si>
+    <t>Desejo que todos os candidatos que foram cadastrados possam ser visualizados em uma Lista</t>
+  </si>
+  <si>
+    <t>Atualizar Eventos de Chamada das telas</t>
+  </si>
+  <si>
+    <t>Desejo que todos os candidatos cadastrados no sistema, sejam visualizados em um lista.</t>
+  </si>
+  <si>
+    <t>Criar Classe ListaCandidatos</t>
+  </si>
+  <si>
+    <t>Integrar Classe ListaCandidatos ao Menu Principal</t>
+  </si>
+  <si>
+    <t>Criar visualização da Lista de Candidatos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -711,14 +740,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -726,9 +755,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,6 +768,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,15 +922,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -948,7 +974,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -997,7 +1023,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
@@ -1110,7 +1136,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1159,7 +1185,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
@@ -1254,11 +1280,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1809067872"/>
-        <c:axId val="1809077120"/>
+        <c:axId val="69953792"/>
+        <c:axId val="69976064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1809067872"/>
+        <c:axId val="69953792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1319,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1809077120"/>
+        <c:crossAx val="69976064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1301,7 +1327,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1809077120"/>
+        <c:axId val="69976064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1347,7 +1373,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1809067872"/>
+        <c:crossAx val="69953792"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1360,6 +1386,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1464,7 +1491,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1499,7 +1526,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1676,7 +1703,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1684,17 +1711,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.42578125"/>
     <col min="2" max="2" width="53.140625"/>
-    <col min="3" max="3" width="49.28515625"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875"/>
     <col min="5" max="5" width="14.140625"/>
     <col min="6" max="6" width="8.85546875"/>
@@ -1702,14 +1729,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1814,10 +1841,10 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1847,8 +1874,8 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="21" t="s">
         <v>55</v>
       </c>
@@ -1876,8 +1903,8 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="22" t="s">
         <v>56</v>
       </c>
@@ -1939,7 +1966,7 @@
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
-      <c r="B9" s="28"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="3" t="s">
         <v>44</v>
       </c>
@@ -1968,7 +1995,7 @@
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32"/>
-      <c r="B10" s="28"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
@@ -1997,7 +2024,7 @@
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
-      <c r="B11" s="28"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
@@ -2026,7 +2053,7 @@
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
       </c>
@@ -2055,7 +2082,7 @@
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
@@ -2084,7 +2111,7 @@
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32"/>
-      <c r="B14" s="28"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="6" t="s">
         <v>43</v>
       </c>
@@ -2113,7 +2140,7 @@
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
-      <c r="B15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="6" t="s">
         <v>42</v>
       </c>
@@ -2141,7 +2168,7 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="38" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="27" t="s">
@@ -2174,8 +2201,8 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="3" t="s">
         <v>59</v>
       </c>
@@ -2203,8 +2230,8 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="6" t="s">
         <v>60</v>
       </c>
@@ -2232,8 +2259,8 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6" t="s">
         <v>61</v>
       </c>
@@ -2261,8 +2288,8 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="6" t="s">
         <v>62</v>
       </c>
@@ -2290,8 +2317,8 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="30"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="6" t="s">
         <v>63</v>
       </c>
@@ -2319,8 +2346,8 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="30"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="6" t="s">
         <v>64</v>
       </c>
@@ -2348,8 +2375,8 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="6" t="s">
         <v>65</v>
       </c>
@@ -2377,8 +2404,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="30"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="4" t="s">
         <v>66</v>
       </c>
@@ -2440,7 +2467,7 @@
     </row>
     <row r="26" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32"/>
-      <c r="B26" s="28"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="23" t="s">
         <v>76</v>
       </c>
@@ -2469,7 +2496,7 @@
     </row>
     <row r="27" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32"/>
-      <c r="B27" s="28"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="23" t="s">
         <v>77</v>
       </c>
@@ -2530,8 +2557,8 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="6" t="s">
         <v>70</v>
       </c>
@@ -2559,8 +2586,8 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="6" t="s">
         <v>71</v>
       </c>
@@ -2588,8 +2615,8 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="24" t="s">
         <v>73</v>
       </c>
@@ -2617,8 +2644,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="24" t="s">
         <v>72</v>
       </c>
@@ -2645,15 +2672,15 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="24" t="s">
         <v>101</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>103</v>
       </c>
       <c r="D33" s="5">
         <v>0.5</v>
@@ -2678,11 +2705,11 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+    <row r="34" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
@@ -2707,11 +2734,11 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
+    <row r="35" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D35" s="5">
         <v>2</v>
@@ -2736,15 +2763,15 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
@@ -2756,11 +2783,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+    <row r="37" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -2772,11 +2799,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+    <row r="38" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D38" s="5">
         <v>1</v>
@@ -2784,13 +2811,15 @@
       <c r="E38" s="5">
         <v>0.5</v>
       </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="F38" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" s="5">
         <v>1.5</v>
@@ -2802,15 +2831,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
         <v>81</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" s="5">
         <v>3</v>
@@ -2822,11 +2851,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
+    <row r="41" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="5">
         <v>0.5</v>
@@ -2838,11 +2867,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
+    <row r="42" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D42" s="5">
         <v>4</v>
@@ -2854,130 +2883,204 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0.83</v>
+      </c>
+      <c r="F43" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="5">
+        <v>1</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="F44" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="5">
+        <v>2</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1.72</v>
+      </c>
+      <c r="F45" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="F46" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="5">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5">
+        <v>1.66</v>
+      </c>
+      <c r="F47" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="5">
+        <v>2</v>
+      </c>
+      <c r="E48" s="5">
+        <v>1.85</v>
+      </c>
+      <c r="F48" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="5">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="F49" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0.87</v>
+      </c>
+      <c r="F50" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E51" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F51" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:19" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
+      <c r="B52" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="C52" s="6"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
+    <row r="53" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="C53" s="6"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="25"/>
-    </row>
-    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="5"/>
@@ -3032,23 +3135,27 @@
       <c r="E61" s="5"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="25"/>
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A62" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="6"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="6"/>
@@ -3091,45 +3198,117 @@
       <c r="F68" s="6"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="6"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="25"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="23">
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A8:A15"/>
     <mergeCell ref="B8:B15"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A40:A42"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="B16:B24"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3143,7 +3322,7 @@
   </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
@@ -3374,31 +3553,31 @@
       </c>
       <c r="F6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="G6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="H6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="I6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="K6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="L6" s="15">
         <f t="shared" si="1"/>
-        <v>406.81670000000003</v>
+        <v>396.03670000000005</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
@@ -3492,7 +3671,7 @@
       </c>
       <c r="F9" s="15">
         <f>SUMIF('Product Backlog'!F:F,4,'Product Backlog'!E:E)</f>
-        <v>11.16</v>
+        <v>21.940000000000005</v>
       </c>
       <c r="G9" s="15">
         <f>SUMIF('Product Backlog'!F:F,5,'Product Backlog'!E:E)</f>
@@ -3520,11 +3699,11 @@
       </c>
       <c r="M9" s="15">
         <f>SUM(C9:L9)</f>
-        <v>93.183300000000003</v>
+        <v>103.9633</v>
       </c>
       <c r="N9" s="15">
         <f>M9/10</f>
-        <v>9.3183299999999996</v>
+        <v>10.396330000000001</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>

</xml_diff>

<commit_message>
Atualização Sprint 4 COMPLETA
</commit_message>
<xml_diff>
--- a/Sprint-4/Product Backlog-Burndown.xlsx
+++ b/Sprint-4/Product Backlog-Burndown.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\PROJETO\adocao\Sprint-4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8145" tabRatio="990"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Product Burndown" sheetId="2" r:id="rId2"/>
     <sheet name="Lista de tarefas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -391,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -490,6 +495,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -663,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -737,15 +749,18 @@
     <xf numFmtId="4" fontId="13" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -773,9 +788,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,6 +804,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,6 +937,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1024,11 +1042,14 @@
           </c:val>
           <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6672-459F-9697-9E0FFD9903C1}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>label 0</c15:sqref>
@@ -1049,7 +1070,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1095,9 +1116,6 @@
                   </c:strRef>
                 </c15:cat>
               </c15:filteredCategoryTitle>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6672-459F-9697-9E0FFD9903C1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1186,11 +1204,14 @@
           </c:val>
           <c:smooth val="0"/>
           <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6672-459F-9697-9E0FFD9903C1}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>label 1</c15:sqref>
@@ -1211,7 +1232,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1258,9 +1279,6 @@
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6672-459F-9697-9E0FFD9903C1}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -1280,11 +1298,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69953792"/>
-        <c:axId val="69976064"/>
+        <c:axId val="-2012087040"/>
+        <c:axId val="-2012085952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69953792"/>
+        <c:axId val="-2012087040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1337,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69976064"/>
+        <c:crossAx val="-2012085952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1345,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69976064"/>
+        <c:axId val="-2012085952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1373,7 +1391,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69953792"/>
+        <c:crossAx val="-2012087040"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1703,7 +1721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1713,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1729,14 +1747,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1841,10 +1859,10 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="34" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -1874,8 +1892,8 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="21" t="s">
         <v>55</v>
       </c>
@@ -1903,8 +1921,8 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="22" t="s">
         <v>56</v>
       </c>
@@ -1932,10 +1950,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1965,7 +1983,7 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="29"/>
       <c r="C9" s="3" t="s">
         <v>44</v>
@@ -1994,7 +2012,7 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>45</v>
@@ -2023,7 +2041,7 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="29"/>
       <c r="C11" s="6" t="s">
         <v>46</v>
@@ -2052,7 +2070,7 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="29"/>
       <c r="C12" s="6" t="s">
         <v>47</v>
@@ -2081,7 +2099,7 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="29"/>
       <c r="C13" s="6" t="s">
         <v>48</v>
@@ -2110,7 +2128,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="29"/>
       <c r="C14" s="6" t="s">
         <v>43</v>
@@ -2139,7 +2157,7 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="29"/>
       <c r="C15" s="6" t="s">
         <v>42</v>
@@ -2168,10 +2186,10 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="28" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -2201,7 +2219,7 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="29"/>
       <c r="C17" s="3" t="s">
         <v>59</v>
@@ -2230,7 +2248,7 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="29"/>
       <c r="C18" s="6" t="s">
         <v>60</v>
@@ -2259,7 +2277,7 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="29"/>
       <c r="C19" s="6" t="s">
         <v>61</v>
@@ -2288,7 +2306,7 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="29"/>
       <c r="C20" s="6" t="s">
         <v>62</v>
@@ -2317,7 +2335,7 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="29"/>
       <c r="C21" s="6" t="s">
         <v>63</v>
@@ -2346,7 +2364,7 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="29"/>
       <c r="C22" s="6" t="s">
         <v>64</v>
@@ -2375,7 +2393,7 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="29"/>
       <c r="C23" s="6" t="s">
         <v>65</v>
@@ -2404,8 +2422,8 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="4" t="s">
         <v>66</v>
       </c>
@@ -2433,10 +2451,10 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="28" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="23" t="s">
@@ -2466,7 +2484,7 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="29"/>
       <c r="C26" s="23" t="s">
         <v>76</v>
@@ -2495,7 +2513,7 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="29"/>
       <c r="C27" s="23" t="s">
         <v>77</v>
@@ -2524,10 +2542,10 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C28" s="23" t="s">
@@ -2644,8 +2662,8 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="24" t="s">
         <v>72</v>
       </c>
@@ -2673,10 +2691,10 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="28" t="s">
         <v>100</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -2735,8 +2753,8 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="24" t="s">
         <v>103</v>
       </c>
@@ -2764,10 +2782,10 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="28" t="s">
         <v>84</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -2816,8 +2834,8 @@
       </c>
     </row>
     <row r="39" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="6" t="s">
         <v>95</v>
       </c>
@@ -2832,10 +2850,10 @@
       </c>
     </row>
     <row r="40" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="28" t="s">
         <v>90</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -2868,8 +2886,8 @@
       </c>
     </row>
     <row r="42" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="3" t="s">
         <v>98</v>
       </c>
@@ -2884,10 +2902,10 @@
       </c>
     </row>
     <row r="43" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="28" t="s">
         <v>108</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2920,8 +2938,8 @@
       </c>
     </row>
     <row r="45" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="3" t="s">
         <v>110</v>
       </c>
@@ -2936,10 +2954,10 @@
       </c>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="28" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2988,10 +3006,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -3024,9 +3042,9 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="4" t="s">
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="27" t="s">
         <v>121</v>
       </c>
       <c r="D51" s="5">
@@ -3286,29 +3304,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A8:A15"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="B16:B24"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
     <mergeCell ref="B36:B39"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="A43:A45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -3387,25 +3405,25 @@
       <c r="E2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="46" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="1"/>
@@ -3425,13 +3443,13 @@
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
       <c r="E3" s="45"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3718,6 +3736,10 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:L8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A2:A3"/>
@@ -3731,10 +3753,6 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:L8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>